<commit_message>
2013-11-22	审批	修复	无法添加 2013-11-22	JS	删除	删除google cdn jquery
</commit_message>
<xml_diff>
--- a/更新日志.xlsx
+++ b/更新日志.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
   <si>
     <t>审批</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -126,6 +126,30 @@
   </si>
   <si>
     <t>-</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>flow</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>emp_no</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>JS</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>删除</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>删除google cdn jquery</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1082,10 +1106,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21.6" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1237,6 +1261,40 @@
         <v>20</v>
       </c>
     </row>
+    <row r="9" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>41600</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>41600</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
2014/5/29	用户	新增	删除用户功能 2014/6/1	系统	改进	附件上传。显示修改为Widget 2014/6/2	系统	改进	CommonAction.class.php CommonModel.class.php
</commit_message>
<xml_diff>
--- a/更新日志.xlsx
+++ b/更新日志.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="145">
   <si>
     <t>日期</t>
   </si>
@@ -566,6 +566,18 @@
   </si>
   <si>
     <t>name</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>删除用户功能</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>CommonAction.class.php CommonModel.class.php</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>附件上传。显示修改为Widget</t>
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
 </sst>
@@ -1502,11 +1514,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G59"/>
+  <dimension ref="A1:G62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D60" sqref="D60"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D67" sqref="D67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2416,6 +2428,48 @@
       </c>
       <c r="G59" s="5" t="s">
         <v>141</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A60" s="8">
+        <v>41788</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D60" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A61" s="8">
+        <v>41791</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="D61" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A62" s="8">
+        <v>41792</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="D62" t="s">
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2014/8/20	流程	改进	添加申请权限	think_flow_type		request_duy,report_duty 2014/8/20	邮件	改进	增加SSL链接功能 2014/8/20	附件	附件	修复不显示添加按钮的BUG
</commit_message>
<xml_diff>
--- a/更新日志.xlsx
+++ b/更新日志.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="179">
   <si>
     <t>日期</t>
   </si>
@@ -722,6 +722,34 @@
   </si>
   <si>
     <t>选择联系人时，出现禁用的员工</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>改进</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>添加申请权限</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>think_flow_type</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>request_duy,report_duty</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>增加SSL链接功能</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>附件</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>修复不显示添加按钮的BUG</t>
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
 </sst>
@@ -1637,11 +1665,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G77"/>
+  <dimension ref="A1:G80"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A76" sqref="A76:D77"/>
+      <selection pane="bottomLeft" activeCell="E80" sqref="E80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2821,6 +2849,54 @@
       </c>
       <c r="D77" s="7" t="s">
         <v>171</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A78" s="5">
+        <v>41871</v>
+      </c>
+      <c r="B78" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="D78" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="E78" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="G78" s="3" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A79" s="5">
+        <v>41871</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="D79" s="7" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A80" s="5">
+        <v>41871</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="D80" s="7" t="s">
+        <v>178</v>
       </c>
     </row>
   </sheetData>

</xml_diff>